<commit_message>
content update fw mar est
</commit_message>
<xml_diff>
--- a/content/species/data/sp_mammals_table3.xlsx
+++ b/content/species/data/sp_mammals_table3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_repos\species\quarto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workflows\NBA\content\species\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194E199A-C1B9-4FF9-A30D-A9F85255E7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2178A13-432D-4590-9812-91634EB7162B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BEC351D-E070-47B5-B73E-49D0C47D7B2D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BEC351D-E070-47B5-B73E-49D0C47D7B2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Recovery project list-Table" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>Volunteer; sponsor GPS collars; school outreach support</t>
   </si>
   <si>
-    <t>Ground pangolin (Smutsia temminckii)</t>
-  </si>
-  <si>
     <t>Black rhinoceros (*Diceros bicornis*)</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>[pangolin.org.za](http://pangolin.org.za)</t>
+  </si>
+  <si>
+    <t>Ground pangolin (*Smutsia temminckii*)</t>
   </si>
 </sst>
 </file>
@@ -599,20 +599,20 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -632,7 +632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -643,16 +643,16 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -663,16 +663,16 @@
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -683,16 +683,16 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -703,16 +703,16 @@
         <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -723,16 +723,16 @@
         <v>24</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -743,16 +743,16 @@
         <v>28</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -763,16 +763,16 @@
         <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
@@ -783,16 +783,16 @@
         <v>35</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -803,10 +803,10 @@
         <v>35</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>38</v>
@@ -831,6 +831,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9251B87A2689245AA9FD86C69F20C58" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c860c8d8cea428af55d2deb18db3c3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de6781d5-cbdf-44cc-b8b1-919d4413b058" xmlns:ns3="d08e37f2-beba-4595-a3e8-aa91f032b3fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1915556badb0c1501ee51a52d85f263" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1108,15 +1117,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B78B7F20-AC4C-4EC2-BDAA-5DF6325624CD}">
   <ds:schemaRefs>
@@ -1130,6 +1130,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BACF3DD1-ECB8-4545-BD4B-F4F35494172F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{301678A8-E84C-46AA-AC62-208143A65756}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1147,12 +1155,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BACF3DD1-ECB8-4545-BD4B-F4F35494172F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>